<commit_message>
gotta save before testing
</commit_message>
<xml_diff>
--- a/digits1.xlsx
+++ b/digits1.xlsx
@@ -393,329 +393,329 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-1.669277608775663</v>
+        <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.499508633382586</v>
+        <v>0</v>
       </c>
       <c r="C1" t="n">
-        <v>-1.158823392505349</v>
+        <v>0</v>
       </c>
       <c r="D1" t="n">
-        <v>0.845768647365746</v>
+        <v>0</v>
       </c>
       <c r="E1" t="n">
-        <v>-1.612178810477517</v>
+        <v>0</v>
       </c>
       <c r="F1" t="n">
-        <v>-1.020209658859805</v>
+        <v>0</v>
       </c>
       <c r="G1" t="n">
-        <v>1.187226522600459</v>
+        <v>0</v>
       </c>
       <c r="H1" t="n">
-        <v>2.075207296806318</v>
+        <v>0</v>
       </c>
       <c r="I1" t="n">
-        <v>0.8138135505488755</v>
+        <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>0.3486794002604874</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.736173808500417</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.6661353158000261</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>2.112510584644715</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.9842553335870136</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.049724017306713</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7029551877183374</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1.041689109942886</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.338845127068497</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>-2.165339745984296</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>-1.608618064869416</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.3661958177660465</v>
+        <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.4207200590628183</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.070742140142051</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1.587108458923901</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1.229272660957686</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1.669627566050758</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4129925192325987</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>2.133143765162692</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.6112959012662093</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.3571582452961825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2.285053197551656</v>
+        <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.4833993710786859</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.01921000479603449</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.2664656486581549</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>-2.344709144599906</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>-2.533963635619769</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>-2.097757520478478</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>-1.866007801787223</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.6939043095373799</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>-1.717968809275445</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.6809298435020231</v>
+        <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>0.4506921671852686</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.1730948158073019</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.4962707102498847</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1.978415259208105</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.06219614038368444</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.06248076095636031</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>2.180153017357891</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.4576372702832899</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4121387060475266</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.5144138966298453</v>
+        <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.1574198856377696</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.5664747204778592</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1.156598243064008</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.3014471980858912</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>-2.441042385227474</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.542787626124538</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.01833133274895017</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.172976549530983</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.4335641401997796</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-2.685127454003159</v>
+        <v>0</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.05880619220118134</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.4237569137522221</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1.2359871398157</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>1.101180502784587</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1.326082876908082</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>2.207378682834726</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>-1.672563070149163</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.4295231491965865</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>0.7972943175123847</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-1.028759632010998</v>
+        <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.30735313458616</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.06075074786865648</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>1.026101593968701</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.601442172505861</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9367267585221147</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.93983166989748</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.9640304075765738</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>1.649340115480099</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>-1.301335623488224</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.007714673252460805</v>
+        <v>0</v>
       </c>
       <c r="B9" t="n">
-        <v>0.4338283456947138</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8493929586597583</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>-2.803992489946479</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>1.46336703656329</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>-1.945977613575455</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>-2.010600776299472</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>2.426665800894804</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.1303656996880046</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.02916235686616789</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-1.770567480109027</v>
+        <v>0</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.9376867018083873</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>-2.295030381747057</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1499180167466374</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.7709103236686623</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>2.529112074933225</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.862944611412057</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>-2.424692282106141</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.1836518531804514</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.0264623700156175</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>